<commit_message>
added 1k graph for testing. Done with measuraments
</commit_message>
<xml_diff>
--- a/doc/mjerenja i grafovi.xlsx
+++ b/doc/mjerenja i grafovi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Razvoj\GitHub\bioinformatics\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B4A8EF8-B9BA-45BA-96BD-23FB2F8E6834}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99561B85-6EE0-4069-A12B-4CAB6D6972BF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="7920" xr2:uid="{8D97927E-20C7-42C1-AF81-9F6E2AA96288}"/>
   </bookViews>
@@ -23,6 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>DULJINA NIZA</t>
   </si>
@@ -39,6 +40,27 @@
   </si>
   <si>
     <t>VRIJEME IZVODENJA</t>
+  </si>
+  <si>
+    <t>10 000 000</t>
+  </si>
+  <si>
+    <t>4 647 121</t>
+  </si>
+  <si>
+    <t>1 000 000</t>
+  </si>
+  <si>
+    <t>100 000</t>
+  </si>
+  <si>
+    <t>10 000</t>
+  </si>
+  <si>
+    <t>1 000</t>
+  </si>
+  <si>
+    <t>AVG (ms)</t>
   </si>
 </sst>
 </file>
@@ -74,8 +96,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalno" xfId="0" builtinId="0"/>
@@ -390,19 +418,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B47DA6A-73C5-4D59-A24E-70600CA49817}">
-  <dimension ref="B2:D2"/>
+  <dimension ref="B2:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.140625" customWidth="1"/>
     <col min="2" max="4" width="30.7109375" customWidth="1"/>
+    <col min="5" max="5" width="25.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -412,8 +441,230 @@
       <c r="D2" t="s">
         <v>2</v>
       </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1">
+        <v>4957</v>
+      </c>
+      <c r="D3" s="2">
+        <v>16219</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="2">
+        <v>16551</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="2">
+        <v>15855</v>
+      </c>
+      <c r="E5">
+        <f>AVERAGE(D3:D5)</f>
+        <v>16208.333333333334</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2448</v>
+      </c>
+      <c r="D6" s="2">
+        <v>8129</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="2">
+        <v>8046</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="2">
+        <v>7983</v>
+      </c>
+      <c r="E8">
+        <f t="shared" ref="E6:E9" si="0">AVERAGE(D6:D8)</f>
+        <v>8052.666666666667</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1">
+        <v>541</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1859</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="2">
+        <v>1762</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="2">
+        <v>1869</v>
+      </c>
+      <c r="E11">
+        <f t="shared" ref="E11" si="1">AVERAGE(D9:D11)</f>
+        <v>1830</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="1">
+        <v>61</v>
+      </c>
+      <c r="D12" s="2">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="2">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="2">
+        <v>167</v>
+      </c>
+      <c r="E14">
+        <f t="shared" ref="E14:E20" si="2">AVERAGE(D12:D14)</f>
+        <v>170.66666666666666</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="1">
+        <v>6</v>
+      </c>
+      <c r="D15" s="2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="2">
+        <v>16</v>
+      </c>
+      <c r="E17">
+        <f t="shared" ref="E17" si="3">AVERAGE(D15:D17)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="D18" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="2">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="1">
+        <v>100</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="D21" s="2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="E23">
+        <f t="shared" ref="E23" si="4">AVERAGE(D21:D23)</f>
+        <v>0.10000000000000002</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="C9:C11"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>